<commit_message>
A lot of version 1.2 tasks & updates
</commit_message>
<xml_diff>
--- a/bin/main/static/template/users.xlsx
+++ b/bin/main/static/template/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maziyar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maziyar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33013252-E28A-4038-87A0-C18322376DB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DF4723-D175-41DC-A7E3-8196C68684B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13710" yWindow="1770" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>userId*</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>09123456789</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>#Parrsoo2020#</t>
+  </si>
+  <si>
+    <t>1400/10/20 13:13:13.259</t>
+  </si>
+  <si>
+    <t>alit</t>
   </si>
 </sst>
 </file>
@@ -122,16 +134,19 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -430,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1000"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -442,10 +457,12 @@
     <col min="6" max="6" width="18.6796875" customWidth="1"/>
     <col min="9" max="9" width="6.7265625" customWidth="1"/>
     <col min="10" max="10" width="15.7265625" customWidth="1"/>
-    <col min="12" max="12" width="42.453125" customWidth="1"/>
+    <col min="11" max="11" width="12.36328125" customWidth="1"/>
+    <col min="12" max="12" width="21.54296875" customWidth="1"/>
+    <col min="13" max="13" width="45.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,13 +496,16 @@
       <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
@@ -514,71 +534,76 @@
       <c r="J2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="L5" s="8" t="s">
+      <c r="M5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="L6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="L7" s="9" t="s">
+      <c r="M7" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B8" s="7"/>
       <c r="D8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="L8" s="9" t="s">
+      <c r="M8" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="L9" s="9" t="s">
+      <c r="M9" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="L10" s="10" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="M10" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="L11" s="10" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="M11" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="L12" s="10" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="M12" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="L13" s="11"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="M13" s="11"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>